<commit_message>
Added temp sensors to arduino pinout
</commit_message>
<xml_diff>
--- a/Documents/Arduino Pinout.xlsx
+++ b/Documents/Arduino Pinout.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Pinout</t>
   </si>
@@ -88,6 +88,18 @@
   </si>
   <si>
     <t>Red LED</t>
+  </si>
+  <si>
+    <t>HLT Temp Sensor</t>
+  </si>
+  <si>
+    <t>MT Temp Sensor</t>
+  </si>
+  <si>
+    <t>BP Temp Sensor</t>
+  </si>
+  <si>
+    <t>Fermenter Temp Sensor</t>
   </si>
 </sst>
 </file>
@@ -428,8 +440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,19 +611,31 @@
       <c r="A26">
         <v>24</v>
       </c>
+      <c r="B26" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
+      <c r="B27" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
+      <c r="B28" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated pinout document to add terminal block numbers for all device ouutputs
</commit_message>
<xml_diff>
--- a/Documents/Arduino Pinout.xlsx
+++ b/Documents/Arduino Pinout.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andersonr\Documents\Autobrew\Documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C55AFF-DB10-484B-9438-7B42329330D7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="90" windowWidth="8595" windowHeight="9270"/>
+    <workbookView xWindow="-15" yWindow="0" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Pinout</t>
   </si>
@@ -100,12 +106,15 @@
   </si>
   <si>
     <t>Fermenter Temp Sensor</t>
+  </si>
+  <si>
+    <t>Terminal Block</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -146,6 +155,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -194,7 +206,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -227,9 +239,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -262,6 +291,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -437,11 +483,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B54"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,197 +495,242 @@
     <col min="2" max="2" width="26.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="B19" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="B20" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="B21" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
       <c r="B22" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
       <c r="B23" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
       <c r="B24" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
       <c r="B25" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
       <c r="B26" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
       <c r="B27" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
       <c r="B28" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
       <c r="B29" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
@@ -647,7 +738,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
@@ -655,7 +746,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
@@ -663,7 +754,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
@@ -671,7 +762,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>32</v>
       </c>
@@ -679,93 +770,114 @@
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
       <c r="B35" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>34</v>
       </c>
       <c r="B36" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>35</v>
       </c>
       <c r="B37" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>36</v>
       </c>
       <c r="B38" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C38">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>37</v>
       </c>
       <c r="B39" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>38</v>
       </c>
       <c r="B40" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C40">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>39</v>
       </c>
       <c r="B41" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C41">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>46</v>
       </c>
@@ -806,7 +918,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -818,7 +930,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Arduino I/O List to include terminal block numbers to be used for all the input/outputs
</commit_message>
<xml_diff>
--- a/Documents/Arduino Pinout.xlsx
+++ b/Documents/Arduino Pinout.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Pinout</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>Fermenter Temp Sensor</t>
+  </si>
+  <si>
+    <t>Terminal Block</t>
   </si>
 </sst>
 </file>
@@ -438,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B54"/>
+  <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,205 +452,253 @@
     <col min="2" max="2" width="26.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="B19" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="B20" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="B21" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
       <c r="B22" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
       <c r="B23" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
       <c r="B24" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
       <c r="B25" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
       <c r="B26" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
       <c r="B27" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
       <c r="B28" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
       <c r="B29" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
       <c r="B30" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C30">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
@@ -655,7 +706,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
@@ -663,7 +714,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
@@ -671,7 +722,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>32</v>
       </c>
@@ -679,93 +730,114 @@
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
       <c r="B35" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>34</v>
       </c>
       <c r="B36" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>35</v>
       </c>
       <c r="B37" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>36</v>
       </c>
       <c r="B38" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C38">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>37</v>
       </c>
       <c r="B39" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>38</v>
       </c>
       <c r="B40" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C40">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>39</v>
       </c>
       <c r="B41" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C41">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>46</v>
       </c>

</xml_diff>

<commit_message>
added a couple documents and update the arduino pinout
</commit_message>
<xml_diff>
--- a/Documents/Arduino Pinout.xlsx
+++ b/Documents/Arduino Pinout.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="35">
   <si>
     <t>Pinout</t>
   </si>
@@ -72,9 +72,6 @@
     <t>HLT Output Flow Sensor</t>
   </si>
   <si>
-    <t>Brewpot Output Flor Sensor</t>
-  </si>
-  <si>
     <t>Pump_Relay</t>
   </si>
   <si>
@@ -103,6 +100,27 @@
   </si>
   <si>
     <t>Terminal Block</t>
+  </si>
+  <si>
+    <t>Voltage Pinout</t>
+  </si>
+  <si>
+    <t>12VDC</t>
+  </si>
+  <si>
+    <t>5VDC</t>
+  </si>
+  <si>
+    <t>I/O</t>
+  </si>
+  <si>
+    <t>OUTPUT</t>
+  </si>
+  <si>
+    <t>Brewpot Output Flow Sensor</t>
+  </si>
+  <si>
+    <t>INPUT</t>
   </si>
 </sst>
 </file>
@@ -126,7 +144,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -134,12 +152,174 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,439 +621,650 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C54"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="9.140625" style="10"/>
     <col min="2" max="2" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="B2" s="1"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="B3" s="1"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="B4" s="1"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="B5" s="1"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="B6" s="1"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="B7" s="1"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="B8" s="1"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="B9" s="1"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="12">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="D10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="8">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="12">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="D11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="8">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="12">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="D12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="8">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="B13" s="1"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="8">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="B14" s="1"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="8">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="B15" s="1"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="8">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="B16" s="1"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="8">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="B17" s="1"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="8">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="B18" s="1"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="8">
         <v>17</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="12">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="D19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="8">
         <v>18</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="12">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="D20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="8">
         <v>19</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="12">
         <v>21</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22">
+      <c r="D21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="8">
         <v>20</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="12">
         <v>17</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23">
+      <c r="D22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="8">
         <v>21</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="12">
         <v>18</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24">
+      <c r="D23" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="8">
         <v>22</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="12">
         <v>15</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25">
+      <c r="D24" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="8">
         <v>23</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="12">
+        <v>16</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="8">
+        <v>24</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="12">
+        <v>11</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="8">
+        <v>25</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="12">
+        <v>12</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="8">
+        <v>26</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="12">
+        <v>13</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="8">
+        <v>27</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" s="12">
+        <v>14</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="8">
+        <v>28</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C25">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>24</v>
-      </c>
-      <c r="B26" t="s">
-        <v>24</v>
-      </c>
-      <c r="C26">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>25</v>
-      </c>
-      <c r="B27" t="s">
-        <v>25</v>
-      </c>
-      <c r="C27">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>26</v>
-      </c>
-      <c r="B28" t="s">
-        <v>26</v>
-      </c>
-      <c r="C28">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>27</v>
-      </c>
-      <c r="B29" t="s">
-        <v>27</v>
-      </c>
-      <c r="C29">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>28</v>
-      </c>
-      <c r="B30" t="s">
+      <c r="C30" s="12">
+        <v>22</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="8">
+        <v>29</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C30">
+      <c r="C31" s="12"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="4"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="8">
+        <v>30</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32" s="12"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="4"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="8">
+        <v>31</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33" s="12"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="4"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="8">
+        <v>32</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31">
+      <c r="C34" s="12"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="4"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="8">
+        <v>33</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C35" s="12">
+        <v>1</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E35" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B31" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>30</v>
-      </c>
-      <c r="B32" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>31</v>
-      </c>
-      <c r="B33" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>32</v>
-      </c>
-      <c r="B34" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>33</v>
-      </c>
-      <c r="B35" t="s">
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="8">
+        <v>34</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" s="12">
         <v>2</v>
       </c>
-      <c r="C35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>34</v>
-      </c>
-      <c r="B36" t="s">
+      <c r="D36" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="8">
+        <v>35</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" s="12">
         <v>3</v>
       </c>
-      <c r="C36">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>35</v>
-      </c>
-      <c r="B37" t="s">
+      <c r="D37" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="8">
+        <v>36</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" s="12">
         <v>4</v>
       </c>
-      <c r="C37">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>36</v>
-      </c>
-      <c r="B38" t="s">
+      <c r="D38" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="8">
+        <v>37</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" s="12">
         <v>5</v>
       </c>
-      <c r="C38">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>37</v>
-      </c>
-      <c r="B39" t="s">
+      <c r="D39" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="8">
+        <v>38</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40" s="12">
         <v>6</v>
       </c>
-      <c r="C39">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>38</v>
-      </c>
-      <c r="B40" t="s">
+      <c r="D40" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="9">
+        <v>39</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" s="13">
         <v>7</v>
       </c>
-      <c r="C40">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>39</v>
-      </c>
-      <c r="B41" t="s">
-        <v>8</v>
-      </c>
-      <c r="C41">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42">
+      <c r="D41" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="10">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43">
+    <row r="43" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="10">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44">
+    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="10">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45">
+    <row r="45" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="10">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46">
+    <row r="46" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="10">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47">
+    <row r="47" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="10">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48">
+    <row r="48" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="10">
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49">
+    <row r="49" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="10">
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50">
+    <row r="50" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="10">
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51">
+    <row r="51" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="10">
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52">
+    <row r="52" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="10">
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53">
+    <row r="53" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="10">
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54">
+    <row r="54" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="10">
         <v>52</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>